<commit_message>
Forecasting: Principles and Practice, the Pythonic Way
</commit_message>
<xml_diff>
--- a/tables/time_series.xlsx
+++ b/tables/time_series.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/materov/ALL/@GitProjects/@2024/rsources-book/tables/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA51B392-1C34-B040-96A2-DA82CF1FDF57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A535159-837C-8648-805D-57D8F9D9AEB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="60" yWindow="500" windowWidth="24940" windowHeight="14180" xr2:uid="{DF9C2308-7DE4-724B-A077-C804DE5E9C7F}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="44">
   <si>
     <t>author</t>
   </si>
@@ -158,6 +158,15 @@
   </si>
   <si>
     <t>https://tidyverts.org/</t>
+  </si>
+  <si>
+    <t>Forecasting: Principles and Practice, the Pythonic Way</t>
+  </si>
+  <si>
+    <t>https://otexts.com/fpppy/</t>
+  </si>
+  <si>
+    <t>Hyndman, R.J., Athanasopoulos, G., Garza, A., Challu, C., Mergenthaler, M., &amp; Olivares, K.G.</t>
   </si>
 </sst>
 </file>
@@ -513,10 +522,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50D566FA-41AC-1743-A66B-6F1FF1535269}">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -603,80 +612,91 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" ht="51" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B9" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C9" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
+    <row r="10" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B10" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C10" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="51" x14ac:dyDescent="0.2">
-      <c r="A10" s="1" t="s">
+    <row r="11" spans="1:3" ht="51" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B11" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C11" s="1" t="s">
         <v>27</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="34" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>12</v>
+        <v>34</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="34" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="34" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B14" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C14" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
+    <row r="15" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B15" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C15" s="1" t="s">
         <v>37</v>
       </c>
     </row>

</xml_diff>